<commit_message>
grafico resumen metas terminado
</commit_message>
<xml_diff>
--- a/backend/resources/templates/LP.xlsx
+++ b/backend/resources/templates/LP.xlsx
@@ -596,7 +596,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -631,6 +631,58 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="8" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="8" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -646,72 +698,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="8" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="8" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -838,9 +844,7 @@
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -896,7 +900,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:ln/>
@@ -1097,7 +1100,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1174,8 +1176,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="-25"/>
-        <c:axId val="301228016"/>
-        <c:axId val="301224208"/>
+        <c:axId val="599360240"/>
+        <c:axId val="496985872"/>
       </c:barChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1227,7 +1229,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1303,11 +1304,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="301229104"/>
-        <c:axId val="301225840"/>
+        <c:axId val="496982608"/>
+        <c:axId val="496983696"/>
       </c:scatterChart>
       <c:catAx>
-        <c:axId val="301228016"/>
+        <c:axId val="599360240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1347,7 +1348,7 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="301224208"/>
+        <c:crossAx val="496985872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1355,7 +1356,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="301224208"/>
+        <c:axId val="496985872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1365,12 +1366,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="301228016"/>
+        <c:crossAx val="599360240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="301225840"/>
+        <c:axId val="496983696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1380,12 +1381,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="301229104"/>
+        <c:crossAx val="496982608"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="301229104"/>
+        <c:axId val="496982608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1394,7 +1395,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="301225840"/>
+        <c:crossAx val="496983696"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1992,55 +1993,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>541727</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>76297</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000AC0D0000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1524000" y="4552950"/>
-          <a:ext cx="10476302" cy="2743297"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
@@ -2395,659 +2347,659 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CD5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="57.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="54.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="40.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="49.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="60.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="14" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="12" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" style="43" customWidth="1"/>
+    <col min="4" max="4" width="60.28515625" style="43" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" style="43" customWidth="1"/>
+    <col min="6" max="6" width="60.5703125" style="43" customWidth="1"/>
+    <col min="7" max="7" width="22" style="43" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.42578125" style="43" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.7109375" style="43" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" style="43" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="49.140625" style="43" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.140625" style="43" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="33.5703125" style="43" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="60.5703125" style="43" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.7109375" style="43" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18" style="43" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.42578125" style="43" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.5703125" style="43" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.42578125" style="43" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.5703125" style="43" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.42578125" style="43" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.5703125" style="43" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.42578125" style="43" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="29.28515625" style="43" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.5703125" style="43" customWidth="1"/>
+    <col min="26" max="26" width="24.5703125" style="43" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.28515625" style="43" customWidth="1"/>
+    <col min="28" max="28" width="11.42578125" style="43" customWidth="1"/>
+    <col min="29" max="29" width="12.5703125" style="43" customWidth="1"/>
+    <col min="30" max="30" width="11" style="43" customWidth="1"/>
+    <col min="31" max="31" width="12.5703125" style="43" customWidth="1"/>
+    <col min="32" max="32" width="13.28515625" style="43" customWidth="1"/>
+    <col min="33" max="33" width="24.42578125" style="43" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="30.28515625" style="43" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.28515625" style="43" customWidth="1"/>
+    <col min="36" max="36" width="24.5703125" style="43" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.28515625" style="43" customWidth="1"/>
+    <col min="38" max="38" width="12.42578125" style="43" customWidth="1"/>
+    <col min="39" max="39" width="13.7109375" style="43" customWidth="1"/>
+    <col min="40" max="40" width="10.7109375" style="43" customWidth="1"/>
+    <col min="41" max="41" width="11.5703125" style="43" customWidth="1"/>
+    <col min="42" max="42" width="12.140625" style="43" customWidth="1"/>
+    <col min="43" max="43" width="25.42578125" style="43" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="31.28515625" style="43" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="11.28515625" style="43" customWidth="1"/>
+    <col min="46" max="46" width="24.5703125" style="43" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.140625" style="43" customWidth="1"/>
+    <col min="48" max="48" width="14.7109375" style="43" customWidth="1"/>
+    <col min="49" max="49" width="13.42578125" style="43" customWidth="1"/>
+    <col min="50" max="50" width="12.85546875" style="43" customWidth="1"/>
+    <col min="51" max="51" width="14.85546875" style="43" customWidth="1"/>
+    <col min="52" max="52" width="15" style="43" customWidth="1"/>
+    <col min="53" max="53" width="25.7109375" style="43" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="24.5703125" style="43" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="11.28515625" style="43" customWidth="1"/>
+    <col min="56" max="56" width="24.5703125" style="43" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="13.5703125" style="43" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="18.28515625" style="43" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="14" style="43" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="12" style="43" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="11.7109375" style="43" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="11.85546875" style="43" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="11.5703125" style="43" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="16.28515625" style="43" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="24.28515625" style="43" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="18.42578125" style="43" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="22.5703125" style="43" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="21" style="43" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:82" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="19"/>
-      <c r="B1" s="19"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
-      <c r="V1" s="20"/>
-      <c r="W1" s="20"/>
-      <c r="X1" s="20"/>
-      <c r="Y1" s="20"/>
-      <c r="Z1" s="20"/>
-      <c r="AA1" s="20"/>
-      <c r="AB1" s="20"/>
-      <c r="AC1" s="20"/>
-      <c r="AD1" s="20"/>
-      <c r="AE1" s="20"/>
-      <c r="AF1" s="20"/>
-      <c r="AG1" s="20"/>
-      <c r="AH1" s="20"/>
-      <c r="AI1" s="20"/>
-      <c r="AJ1" s="20"/>
-      <c r="AK1" s="20"/>
-      <c r="AL1" s="20"/>
-      <c r="AM1" s="20"/>
-      <c r="AN1" s="20"/>
-      <c r="AO1" s="20"/>
-      <c r="AP1" s="20"/>
-      <c r="AQ1" s="20"/>
-      <c r="AR1" s="20"/>
-      <c r="AS1" s="20"/>
-      <c r="AT1" s="20"/>
-      <c r="AU1" s="20"/>
-      <c r="AV1" s="20"/>
-      <c r="AW1" s="20"/>
-      <c r="AX1" s="20"/>
-      <c r="AY1" s="20"/>
-      <c r="AZ1" s="20"/>
-      <c r="BA1" s="20"/>
-      <c r="BB1" s="20"/>
-      <c r="BC1" s="20"/>
-      <c r="BD1" s="20"/>
-      <c r="BE1" s="19"/>
-      <c r="BF1" s="22"/>
-      <c r="BG1" s="19"/>
-      <c r="BH1" s="19"/>
-      <c r="BI1" s="19"/>
-      <c r="BJ1" s="19"/>
-      <c r="BK1" s="19"/>
-      <c r="BL1" s="19"/>
-      <c r="BM1" s="19"/>
-      <c r="BN1" s="19"/>
-      <c r="BO1" s="19"/>
-      <c r="BP1" s="19"/>
-      <c r="BQ1" s="19"/>
-      <c r="BR1" s="19"/>
-      <c r="BS1" s="19"/>
-      <c r="BT1" s="19"/>
-      <c r="BU1" s="19"/>
-      <c r="BV1" s="19"/>
-      <c r="BW1" s="19"/>
-      <c r="BX1" s="19"/>
-      <c r="BY1" s="19"/>
-      <c r="BZ1" s="19"/>
-      <c r="CA1" s="19"/>
-      <c r="CB1" s="19"/>
-      <c r="CC1" s="19"/>
-      <c r="CD1" s="19"/>
+      <c r="A1" s="14"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
+      <c r="W1" s="37"/>
+      <c r="X1" s="37"/>
+      <c r="Y1" s="37"/>
+      <c r="Z1" s="37"/>
+      <c r="AA1" s="37"/>
+      <c r="AB1" s="37"/>
+      <c r="AC1" s="37"/>
+      <c r="AD1" s="37"/>
+      <c r="AE1" s="37"/>
+      <c r="AF1" s="37"/>
+      <c r="AG1" s="37"/>
+      <c r="AH1" s="37"/>
+      <c r="AI1" s="37"/>
+      <c r="AJ1" s="37"/>
+      <c r="AK1" s="37"/>
+      <c r="AL1" s="37"/>
+      <c r="AM1" s="37"/>
+      <c r="AN1" s="37"/>
+      <c r="AO1" s="37"/>
+      <c r="AP1" s="37"/>
+      <c r="AQ1" s="37"/>
+      <c r="AR1" s="37"/>
+      <c r="AS1" s="37"/>
+      <c r="AT1" s="37"/>
+      <c r="AU1" s="37"/>
+      <c r="AV1" s="37"/>
+      <c r="AW1" s="37"/>
+      <c r="AX1" s="37"/>
+      <c r="AY1" s="37"/>
+      <c r="AZ1" s="37"/>
+      <c r="BA1" s="37"/>
+      <c r="BB1" s="37"/>
+      <c r="BC1" s="37"/>
+      <c r="BD1" s="37"/>
+      <c r="BE1" s="39"/>
+      <c r="BF1" s="40"/>
+      <c r="BG1" s="39"/>
+      <c r="BH1" s="39"/>
+      <c r="BI1" s="39"/>
+      <c r="BJ1" s="39"/>
+      <c r="BK1" s="39"/>
+      <c r="BL1" s="39"/>
+      <c r="BM1" s="39"/>
+      <c r="BN1" s="39"/>
+      <c r="BO1" s="39"/>
+      <c r="BP1" s="39"/>
+      <c r="BQ1" s="14"/>
+      <c r="BR1" s="14"/>
+      <c r="BS1" s="14"/>
+      <c r="BT1" s="14"/>
+      <c r="BU1" s="14"/>
+      <c r="BV1" s="14"/>
+      <c r="BW1" s="14"/>
+      <c r="BX1" s="14"/>
+      <c r="BY1" s="14"/>
+      <c r="BZ1" s="14"/>
+      <c r="CA1" s="14"/>
+      <c r="CB1" s="14"/>
+      <c r="CC1" s="14"/>
+      <c r="CD1" s="14"/>
     </row>
     <row r="2" spans="1:82" ht="41.25" x14ac:dyDescent="0.35">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="23" t="s">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="23"/>
-      <c r="S2" s="23"/>
-      <c r="T2" s="23"/>
-      <c r="U2" s="23"/>
-      <c r="V2" s="23"/>
-      <c r="W2" s="23"/>
-      <c r="X2" s="23"/>
-      <c r="Y2" s="23"/>
-      <c r="Z2" s="23"/>
-      <c r="AA2" s="23"/>
-      <c r="AB2" s="23"/>
-      <c r="AC2" s="23"/>
-      <c r="AD2" s="23"/>
-      <c r="AE2" s="23"/>
-      <c r="AF2" s="23"/>
-      <c r="AG2" s="23"/>
-      <c r="AH2" s="23"/>
-      <c r="AI2" s="23"/>
-      <c r="AJ2" s="23"/>
-      <c r="AK2" s="23"/>
-      <c r="AL2" s="23"/>
-      <c r="AM2" s="23"/>
-      <c r="AN2" s="23"/>
-      <c r="AO2" s="23"/>
-      <c r="AP2" s="23"/>
-      <c r="AQ2" s="23"/>
-      <c r="AR2" s="23"/>
-      <c r="AS2" s="23"/>
-      <c r="AT2" s="23"/>
-      <c r="AU2" s="23"/>
-      <c r="AV2" s="23"/>
-      <c r="AW2" s="23"/>
-      <c r="AX2" s="23"/>
-      <c r="AY2" s="23"/>
-      <c r="AZ2" s="23"/>
-      <c r="BA2" s="23"/>
-      <c r="BB2" s="23"/>
-      <c r="BC2" s="23"/>
-      <c r="BD2" s="23"/>
-      <c r="BE2" s="23"/>
-      <c r="BF2" s="23"/>
-      <c r="BG2" s="23"/>
-      <c r="BH2" s="23"/>
-      <c r="BI2" s="23"/>
-      <c r="BJ2" s="23"/>
-      <c r="BK2" s="23"/>
-      <c r="BL2" s="23"/>
-      <c r="BM2" s="23"/>
-      <c r="BN2" s="23"/>
-      <c r="BO2" s="23"/>
-      <c r="BP2" s="23"/>
-      <c r="BQ2" s="19"/>
-      <c r="BR2" s="19"/>
-      <c r="BS2" s="19"/>
-      <c r="BT2" s="19"/>
-      <c r="BU2" s="19"/>
-      <c r="BV2" s="19"/>
-      <c r="BW2" s="19"/>
-      <c r="BX2" s="19"/>
-      <c r="BY2" s="19"/>
-      <c r="BZ2" s="19"/>
-      <c r="CA2" s="19"/>
-      <c r="CB2" s="19"/>
-      <c r="CC2" s="19"/>
-      <c r="CD2" s="19"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="41"/>
+      <c r="P2" s="41"/>
+      <c r="Q2" s="41"/>
+      <c r="R2" s="41"/>
+      <c r="S2" s="41"/>
+      <c r="T2" s="41"/>
+      <c r="U2" s="41"/>
+      <c r="V2" s="41"/>
+      <c r="W2" s="41"/>
+      <c r="X2" s="41"/>
+      <c r="Y2" s="41"/>
+      <c r="Z2" s="41"/>
+      <c r="AA2" s="41"/>
+      <c r="AB2" s="41"/>
+      <c r="AC2" s="41"/>
+      <c r="AD2" s="41"/>
+      <c r="AE2" s="41"/>
+      <c r="AF2" s="41"/>
+      <c r="AG2" s="41"/>
+      <c r="AH2" s="41"/>
+      <c r="AI2" s="41"/>
+      <c r="AJ2" s="41"/>
+      <c r="AK2" s="41"/>
+      <c r="AL2" s="41"/>
+      <c r="AM2" s="41"/>
+      <c r="AN2" s="41"/>
+      <c r="AO2" s="41"/>
+      <c r="AP2" s="41"/>
+      <c r="AQ2" s="41"/>
+      <c r="AR2" s="41"/>
+      <c r="AS2" s="41"/>
+      <c r="AT2" s="41"/>
+      <c r="AU2" s="41"/>
+      <c r="AV2" s="41"/>
+      <c r="AW2" s="41"/>
+      <c r="AX2" s="41"/>
+      <c r="AY2" s="41"/>
+      <c r="AZ2" s="41"/>
+      <c r="BA2" s="41"/>
+      <c r="BB2" s="41"/>
+      <c r="BC2" s="41"/>
+      <c r="BD2" s="41"/>
+      <c r="BE2" s="41"/>
+      <c r="BF2" s="41"/>
+      <c r="BG2" s="41"/>
+      <c r="BH2" s="41"/>
+      <c r="BI2" s="41"/>
+      <c r="BJ2" s="41"/>
+      <c r="BK2" s="41"/>
+      <c r="BL2" s="41"/>
+      <c r="BM2" s="41"/>
+      <c r="BN2" s="41"/>
+      <c r="BO2" s="41"/>
+      <c r="BP2" s="41"/>
+      <c r="BQ2" s="14"/>
+      <c r="BR2" s="14"/>
+      <c r="BS2" s="14"/>
+      <c r="BT2" s="14"/>
+      <c r="BU2" s="14"/>
+      <c r="BV2" s="14"/>
+      <c r="BW2" s="14"/>
+      <c r="BX2" s="14"/>
+      <c r="BY2" s="14"/>
+      <c r="BZ2" s="14"/>
+      <c r="CA2" s="14"/>
+      <c r="CB2" s="14"/>
+      <c r="CC2" s="14"/>
+      <c r="CD2" s="14"/>
     </row>
     <row r="3" spans="1:82" ht="42" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="24"/>
-      <c r="U3" s="24"/>
-      <c r="V3" s="24"/>
-      <c r="W3" s="24"/>
-      <c r="X3" s="24"/>
-      <c r="Y3" s="24"/>
-      <c r="Z3" s="24"/>
-      <c r="AA3" s="24"/>
-      <c r="AB3" s="24"/>
-      <c r="AC3" s="24"/>
-      <c r="AD3" s="24"/>
-      <c r="AE3" s="24"/>
-      <c r="AF3" s="24"/>
-      <c r="AG3" s="24"/>
-      <c r="AH3" s="24"/>
-      <c r="AI3" s="24"/>
-      <c r="AJ3" s="24"/>
-      <c r="AK3" s="24"/>
-      <c r="AL3" s="24"/>
-      <c r="AM3" s="24"/>
-      <c r="AN3" s="24"/>
-      <c r="AO3" s="24"/>
-      <c r="AP3" s="24"/>
-      <c r="AQ3" s="24"/>
-      <c r="AR3" s="24"/>
-      <c r="AS3" s="24"/>
-      <c r="AT3" s="24"/>
-      <c r="AU3" s="24"/>
-      <c r="AV3" s="24"/>
-      <c r="AW3" s="24"/>
-      <c r="AX3" s="24"/>
-      <c r="AY3" s="24"/>
-      <c r="AZ3" s="24"/>
-      <c r="BA3" s="24"/>
-      <c r="BB3" s="24"/>
-      <c r="BC3" s="24"/>
-      <c r="BD3" s="24"/>
-      <c r="BE3" s="24"/>
-      <c r="BF3" s="24"/>
-      <c r="BG3" s="24"/>
-      <c r="BH3" s="24"/>
-      <c r="BI3" s="24"/>
-      <c r="BJ3" s="24"/>
-      <c r="BK3" s="24"/>
-      <c r="BL3" s="24"/>
-      <c r="BM3" s="24"/>
-      <c r="BN3" s="24"/>
-      <c r="BO3" s="24"/>
-      <c r="BP3" s="24"/>
-      <c r="BQ3" s="19"/>
-      <c r="BR3" s="19"/>
-      <c r="BS3" s="19"/>
-      <c r="BT3" s="19"/>
-      <c r="BU3" s="19"/>
-      <c r="BV3" s="19"/>
-      <c r="BW3" s="19"/>
-      <c r="BX3" s="19"/>
-      <c r="BY3" s="19"/>
-      <c r="BZ3" s="19"/>
-      <c r="CA3" s="19"/>
-      <c r="CB3" s="19"/>
-      <c r="CC3" s="19"/>
-      <c r="CD3" s="19"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="42"/>
+      <c r="P3" s="42"/>
+      <c r="Q3" s="42"/>
+      <c r="R3" s="42"/>
+      <c r="S3" s="42"/>
+      <c r="T3" s="42"/>
+      <c r="U3" s="42"/>
+      <c r="V3" s="42"/>
+      <c r="W3" s="42"/>
+      <c r="X3" s="42"/>
+      <c r="Y3" s="42"/>
+      <c r="Z3" s="42"/>
+      <c r="AA3" s="42"/>
+      <c r="AB3" s="42"/>
+      <c r="AC3" s="42"/>
+      <c r="AD3" s="42"/>
+      <c r="AE3" s="42"/>
+      <c r="AF3" s="42"/>
+      <c r="AG3" s="42"/>
+      <c r="AH3" s="42"/>
+      <c r="AI3" s="42"/>
+      <c r="AJ3" s="42"/>
+      <c r="AK3" s="42"/>
+      <c r="AL3" s="42"/>
+      <c r="AM3" s="42"/>
+      <c r="AN3" s="42"/>
+      <c r="AO3" s="42"/>
+      <c r="AP3" s="42"/>
+      <c r="AQ3" s="42"/>
+      <c r="AR3" s="42"/>
+      <c r="AS3" s="42"/>
+      <c r="AT3" s="42"/>
+      <c r="AU3" s="42"/>
+      <c r="AV3" s="42"/>
+      <c r="AW3" s="42"/>
+      <c r="AX3" s="42"/>
+      <c r="AY3" s="42"/>
+      <c r="AZ3" s="42"/>
+      <c r="BA3" s="42"/>
+      <c r="BB3" s="42"/>
+      <c r="BC3" s="42"/>
+      <c r="BD3" s="42"/>
+      <c r="BE3" s="42"/>
+      <c r="BF3" s="42"/>
+      <c r="BG3" s="42"/>
+      <c r="BH3" s="42"/>
+      <c r="BI3" s="42"/>
+      <c r="BJ3" s="42"/>
+      <c r="BK3" s="42"/>
+      <c r="BL3" s="42"/>
+      <c r="BM3" s="42"/>
+      <c r="BN3" s="42"/>
+      <c r="BO3" s="42"/>
+      <c r="BP3" s="42"/>
+      <c r="BQ3" s="14"/>
+      <c r="BR3" s="14"/>
+      <c r="BS3" s="14"/>
+      <c r="BT3" s="14"/>
+      <c r="BU3" s="14"/>
+      <c r="BV3" s="14"/>
+      <c r="BW3" s="14"/>
+      <c r="BX3" s="14"/>
+      <c r="BY3" s="14"/>
+      <c r="BZ3" s="14"/>
+      <c r="CA3" s="14"/>
+      <c r="CB3" s="14"/>
+      <c r="CC3" s="14"/>
+      <c r="CD3" s="14"/>
     </row>
     <row r="4" spans="1:82" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A4" s="19"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="25" t="s">
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="25" t="s">
+      <c r="G4" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="H4" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="25" t="s">
+      <c r="I4" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="25" t="s">
+      <c r="K4" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="25" t="s">
+      <c r="M4" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="N4" s="25" t="s">
+      <c r="N4" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="O4" s="25" t="s">
+      <c r="O4" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="25" t="s">
+      <c r="P4" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="Q4" s="26" t="s">
+      <c r="Q4" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="R4" s="27"/>
-      <c r="S4" s="27" t="s">
+      <c r="R4" s="25"/>
+      <c r="S4" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="T4" s="27"/>
-      <c r="U4" s="27" t="s">
+      <c r="T4" s="25"/>
+      <c r="U4" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="V4" s="27"/>
-      <c r="W4" s="28" t="s">
+      <c r="V4" s="25"/>
+      <c r="W4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="X4" s="28" t="s">
+      <c r="X4" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="Y4" s="28" t="s">
+      <c r="Y4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="Z4" s="28" t="s">
+      <c r="Z4" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="AA4" s="27" t="s">
+      <c r="AA4" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="AB4" s="27"/>
-      <c r="AC4" s="27" t="s">
+      <c r="AB4" s="25"/>
+      <c r="AC4" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="AD4" s="27"/>
-      <c r="AE4" s="27" t="s">
+      <c r="AD4" s="25"/>
+      <c r="AE4" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="AF4" s="27"/>
-      <c r="AG4" s="28" t="s">
+      <c r="AF4" s="25"/>
+      <c r="AG4" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="AH4" s="28" t="s">
+      <c r="AH4" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="AI4" s="28" t="s">
+      <c r="AI4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="AJ4" s="28" t="s">
+      <c r="AJ4" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="AK4" s="27" t="s">
+      <c r="AK4" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="AL4" s="27"/>
-      <c r="AM4" s="27" t="s">
+      <c r="AL4" s="25"/>
+      <c r="AM4" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="AN4" s="27"/>
-      <c r="AO4" s="27" t="s">
+      <c r="AN4" s="25"/>
+      <c r="AO4" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="AP4" s="27"/>
-      <c r="AQ4" s="28" t="s">
+      <c r="AP4" s="25"/>
+      <c r="AQ4" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="AR4" s="28" t="s">
+      <c r="AR4" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="AS4" s="28" t="s">
+      <c r="AS4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="AT4" s="28" t="s">
+      <c r="AT4" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="AU4" s="27" t="s">
+      <c r="AU4" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="AV4" s="27"/>
-      <c r="AW4" s="27" t="s">
+      <c r="AV4" s="25"/>
+      <c r="AW4" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="AX4" s="27"/>
-      <c r="AY4" s="27" t="s">
+      <c r="AX4" s="25"/>
+      <c r="AY4" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="AZ4" s="29"/>
-      <c r="BA4" s="30" t="s">
+      <c r="AZ4" s="31"/>
+      <c r="BA4" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="BB4" s="30" t="s">
+      <c r="BB4" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="BC4" s="30" t="s">
+      <c r="BC4" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="BD4" s="31" t="s">
+      <c r="BD4" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="BE4" s="32" t="s">
+      <c r="BE4" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="BF4" s="32"/>
-      <c r="BG4" s="32"/>
-      <c r="BH4" s="32"/>
-      <c r="BI4" s="32"/>
-      <c r="BJ4" s="32"/>
-      <c r="BK4" s="32"/>
-      <c r="BL4" s="32"/>
-      <c r="BM4" s="32"/>
-      <c r="BN4" s="32"/>
-      <c r="BO4" s="32"/>
-      <c r="BP4" s="32"/>
-      <c r="BQ4" s="19"/>
-      <c r="BR4" s="19"/>
-      <c r="BS4" s="19"/>
-      <c r="BT4" s="19"/>
-      <c r="BU4" s="19"/>
-      <c r="BV4" s="19"/>
-      <c r="BW4" s="19"/>
-      <c r="BX4" s="19"/>
-      <c r="BY4" s="19"/>
-      <c r="BZ4" s="19"/>
-      <c r="CA4" s="19"/>
-      <c r="CB4" s="19"/>
-      <c r="CC4" s="19"/>
-      <c r="CD4" s="19"/>
+      <c r="BF4" s="30"/>
+      <c r="BG4" s="30"/>
+      <c r="BH4" s="30"/>
+      <c r="BI4" s="30"/>
+      <c r="BJ4" s="30"/>
+      <c r="BK4" s="30"/>
+      <c r="BL4" s="30"/>
+      <c r="BM4" s="30"/>
+      <c r="BN4" s="30"/>
+      <c r="BO4" s="30"/>
+      <c r="BP4" s="30"/>
+      <c r="BQ4" s="14"/>
+      <c r="BR4" s="14"/>
+      <c r="BS4" s="14"/>
+      <c r="BT4" s="14"/>
+      <c r="BU4" s="14"/>
+      <c r="BV4" s="14"/>
+      <c r="BW4" s="14"/>
+      <c r="BX4" s="14"/>
+      <c r="BY4" s="14"/>
+      <c r="BZ4" s="14"/>
+      <c r="CA4" s="14"/>
+      <c r="CB4" s="14"/>
+      <c r="CC4" s="14"/>
+      <c r="CD4" s="14"/>
     </row>
     <row r="5" spans="1:82" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="19"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33"/>
-      <c r="O5" s="33"/>
-      <c r="P5" s="33"/>
-      <c r="Q5" s="34" t="s">
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="R5" s="35" t="s">
+      <c r="R5" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="S5" s="36" t="s">
+      <c r="S5" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="T5" s="35" t="s">
+      <c r="T5" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="U5" s="36" t="s">
+      <c r="U5" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="V5" s="35" t="s">
+      <c r="V5" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="W5" s="37"/>
-      <c r="X5" s="37"/>
-      <c r="Y5" s="37"/>
-      <c r="Z5" s="37"/>
-      <c r="AA5" s="36" t="s">
+      <c r="W5" s="23"/>
+      <c r="X5" s="23"/>
+      <c r="Y5" s="23"/>
+      <c r="Z5" s="23"/>
+      <c r="AA5" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="AB5" s="35" t="s">
+      <c r="AB5" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="AC5" s="36" t="s">
+      <c r="AC5" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="AD5" s="35" t="s">
+      <c r="AD5" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="AE5" s="36" t="s">
+      <c r="AE5" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="AF5" s="35" t="s">
+      <c r="AF5" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="AG5" s="37"/>
-      <c r="AH5" s="37"/>
-      <c r="AI5" s="37"/>
-      <c r="AJ5" s="37"/>
-      <c r="AK5" s="36" t="s">
+      <c r="AG5" s="23"/>
+      <c r="AH5" s="23"/>
+      <c r="AI5" s="23"/>
+      <c r="AJ5" s="23"/>
+      <c r="AK5" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="AL5" s="35" t="s">
+      <c r="AL5" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="AM5" s="36" t="s">
+      <c r="AM5" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="AN5" s="35" t="s">
+      <c r="AN5" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="AO5" s="36" t="s">
+      <c r="AO5" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="AP5" s="35" t="s">
+      <c r="AP5" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="AQ5" s="37"/>
-      <c r="AR5" s="37"/>
-      <c r="AS5" s="37"/>
-      <c r="AT5" s="37"/>
-      <c r="AU5" s="36" t="s">
+      <c r="AQ5" s="23"/>
+      <c r="AR5" s="23"/>
+      <c r="AS5" s="23"/>
+      <c r="AT5" s="23"/>
+      <c r="AU5" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="AV5" s="35" t="s">
+      <c r="AV5" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="AW5" s="36" t="s">
+      <c r="AW5" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="AX5" s="35" t="s">
+      <c r="AX5" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="AY5" s="36" t="s">
+      <c r="AY5" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="AZ5" s="38" t="s">
+      <c r="AZ5" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="BA5" s="39"/>
-      <c r="BB5" s="39"/>
-      <c r="BC5" s="39"/>
-      <c r="BD5" s="40"/>
-      <c r="BE5" s="41" t="s">
+      <c r="BA5" s="27"/>
+      <c r="BB5" s="27"/>
+      <c r="BC5" s="27"/>
+      <c r="BD5" s="29"/>
+      <c r="BE5" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="BF5" s="41" t="s">
+      <c r="BF5" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="BG5" s="41" t="s">
+      <c r="BG5" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="BH5" s="41" t="s">
+      <c r="BH5" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="BI5" s="41" t="s">
+      <c r="BI5" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="BJ5" s="41" t="s">
+      <c r="BJ5" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="BK5" s="41" t="s">
+      <c r="BK5" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="BL5" s="41" t="s">
+      <c r="BL5" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="BM5" s="41" t="s">
+      <c r="BM5" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="BN5" s="41" t="s">
+      <c r="BN5" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="BO5" s="41" t="s">
+      <c r="BO5" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="BP5" s="41" t="s">
+      <c r="BP5" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="BQ5" s="19"/>
-      <c r="BR5" s="19"/>
-      <c r="BS5" s="19"/>
-      <c r="BT5" s="19"/>
-      <c r="BU5" s="19"/>
-      <c r="BV5" s="19"/>
-      <c r="BW5" s="19"/>
-      <c r="BX5" s="19"/>
-      <c r="BY5" s="19"/>
-      <c r="BZ5" s="19"/>
-      <c r="CA5" s="19"/>
-      <c r="CB5" s="19"/>
-      <c r="CC5" s="19"/>
-      <c r="CD5" s="19"/>
+      <c r="BQ5" s="14"/>
+      <c r="BR5" s="14"/>
+      <c r="BS5" s="14"/>
+      <c r="BT5" s="14"/>
+      <c r="BU5" s="14"/>
+      <c r="BV5" s="14"/>
+      <c r="BW5" s="14"/>
+      <c r="BX5" s="14"/>
+      <c r="BY5" s="14"/>
+      <c r="BZ5" s="14"/>
+      <c r="CA5" s="14"/>
+      <c r="CB5" s="14"/>
+      <c r="CC5" s="14"/>
+      <c r="CD5" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="44">
@@ -3061,11 +3013,7 @@
     <mergeCell ref="AW4:AX4"/>
     <mergeCell ref="AY4:AZ4"/>
     <mergeCell ref="BA4:BA5"/>
-    <mergeCell ref="AJ4:AJ5"/>
-    <mergeCell ref="AK4:AL4"/>
-    <mergeCell ref="AM4:AN4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AQ4:AQ5"/>
+    <mergeCell ref="Y4:Y5"/>
     <mergeCell ref="AR4:AR5"/>
     <mergeCell ref="AA4:AB4"/>
     <mergeCell ref="AC4:AD4"/>
@@ -3073,18 +3021,16 @@
     <mergeCell ref="AG4:AG5"/>
     <mergeCell ref="AH4:AH5"/>
     <mergeCell ref="AI4:AI5"/>
+    <mergeCell ref="AJ4:AJ5"/>
+    <mergeCell ref="AK4:AL4"/>
+    <mergeCell ref="AM4:AN4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AQ4:AQ5"/>
+    <mergeCell ref="Q4:R4"/>
     <mergeCell ref="S4:T4"/>
     <mergeCell ref="U4:V4"/>
     <mergeCell ref="W4:W5"/>
     <mergeCell ref="X4:X5"/>
-    <mergeCell ref="Y4:Y5"/>
-    <mergeCell ref="Z4:Z5"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:R4"/>
     <mergeCell ref="H2:BP2"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
@@ -3095,9 +3041,14 @@
     <mergeCell ref="I4:I5"/>
     <mergeCell ref="J4:J5"/>
     <mergeCell ref="K4:K5"/>
+    <mergeCell ref="Z4:Z5"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="P4:P5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3139,24 +3090,24 @@
       <c r="R2" s="1"/>
     </row>
     <row r="3" spans="2:18" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="17"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="33"/>
+      <c r="P3" s="34"/>
+      <c r="Q3" s="35"/>
       <c r="R3" s="1"/>
     </row>
     <row r="4" spans="2:18" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3181,20 +3132,20 @@
     <row r="5" spans="2:18" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="18" t="s">
+      <c r="L5" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="M5" s="18"/>
+      <c r="M5" s="36"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="1"/>

</xml_diff>